<commit_message>
add mave-nn to selected papers
</commit_message>
<xml_diff>
--- a/backend/selected_publications.xlsx
+++ b/backend/selected_publications.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cshl0-my.sharepoint.com/personal/aicorder_cshl_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aicorder\Documents\GitHub\aidancordero2.github.io\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{DE8F2995-19FB-4B5E-A628-B39CAF64227A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E7BAE8F-C9AD-4075-8015-4C4849F0B1F4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE953460-30AE-4091-9C05-C0068FB74CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{5561A58E-8F97-4914-856A-96AEC28CEECE}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Title</t>
   </si>
@@ -109,9 +109,6 @@
     <t>https://www.nature.com/articles/s41467-024-46090-5</t>
   </si>
   <si>
-    <t>This paper introduces an operator algebra framework that bridges two previously disconnected approaches to modeling multiparticle complexes in stochastic chemical systems: the statistical physics formalism (rooted in Doi's 1976 Fock space approach) and rule-based computational methods developed for simulating biochemical complexes. The new formalism extends Fock space to support not just particle creation and annihilation but also the assembly and disassembly of multiparticle complexes, with rules specified by algebraic operators via Wick's theorem and aided by diagrammatic tools. The result is a unified mathematical and computational framework applicable to both equilibrium and nonequilibrium systems, including a stochastic simulation algorithm for the latter.</t>
-  </si>
-  <si>
     <t>https://www.pnas.org/doi/10.1073/pnas.1004290107</t>
   </si>
   <si>
@@ -125,6 +122,24 @@
   </si>
   <si>
     <t>Proceedings of the National Academy of Sciences USA 107 (20)</t>
+  </si>
+  <si>
+    <t>MAVE-NN: learning genotype-phenotype maps from multiplex assays of variant effect</t>
+  </si>
+  <si>
+    <t>Ammar Tareen, Mahdi Kooshkbaghi, Anna Posfai, William T Ireland, David M McCandlish, Justin B Kinney</t>
+  </si>
+  <si>
+    <t>Genome biology 23 (1), 98, 2022</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1186/s13059-022-02661-7</t>
+  </si>
+  <si>
+    <t>hey</t>
+  </si>
+  <si>
+    <t>WOW! This paper introduces an operator algebra framework that bridges two previously disconnected approaches to modeling multiparticle complexes in stochastic chemical systems: the statistical physics formalism (rooted in Doi's 1976 Fock space approach) and rule-based computational methods developed for simulating biochemical complexes. The new formalism extends Fock space to support not just particle creation and annihilation but also the assembly and disassembly of multiparticle complexes, with rules specified by algebraic operators via Wick's theorem and aided by diagrammatic tools. The result is a unified mathematical and computational framework applicable to both equilibrium and nonequilibrium systems, including a stochastic simulation algorithm for the latter.</t>
   </si>
 </sst>
 </file>
@@ -617,9 +632,8 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
@@ -678,10 +692,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1004,7 +1014,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1019,25 +1029,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1058,7 +1068,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1081,7 +1091,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1129,30 +1139,45 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6">
-        <v>2010</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
+        <v>2022</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>2010</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1167,7 +1192,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" xr:uid="{CBAE7786-D596-4808-808C-FF3BA45ADE62}"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{CBAE7786-D596-4808-808C-FF3BA45ADE62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add more paper descriptions
</commit_message>
<xml_diff>
--- a/backend/selected_publications.xlsx
+++ b/backend/selected_publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aicorder\Documents\GitHub\aidancordero2.github.io\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC5739A-E30D-44D3-AE14-483C0AA0C51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C35D392-CCC1-488E-9265-365992444D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{5561A58E-8F97-4914-856A-96AEC28CEECE}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Title</t>
   </si>
@@ -112,9 +112,6 @@
     <t>https://www.pnas.org/doi/10.1073/pnas.1004290107</t>
   </si>
   <si>
-    <t>/pictures/figures/fig1_deeplearning_kinney2010.jpg</t>
-  </si>
-  <si>
     <t>This paper presents a method for quantitatively characterizing the protein-DNA and protein-protein interactions that regulate transcription in living cells, using a library of partially mutated regulatory sequences sorted by transcriptional activity and sequenced in bulk. Computational analysis of the resulting data — enabled by a relationship between likelihood and mutual information — can extract precise biophysical parameters even in the presence of experimental noise. Applied to the E. coli lac promoter, the approach successfully identified binding sites, determined sequence-dependent binding energies, and measured in vivo interaction energies between RNA polymerase and transcription factors.</t>
   </si>
   <si>
@@ -203,6 +200,27 @@
   </si>
   <si>
     <t>Here we introduce Logomaker, a Python API for creating publication-quality sequence logos. Logomaker can produce both standard and highly customized logos from either a matrix-like array of numbers or a multiple-sequence alignment. Logos are rendered as native matplotlib objects that are easy to stylize and incorporate into multi-panel figures.</t>
+  </si>
+  <si>
+    <t>This paper introduces SQUID (Surrogate Quantitative Interpretability for Deepnets), a framework for interpreting genomic deep neural networks by approximating them locally with simpler, inherently interpretable surrogate models that incorporate domain-specific knowledge about cis-regulatory mechanisms. By accounting for the confounding effects of nonlinearities and heteroscedastic noise in functional genomics data, SQUID outperforms existing interpretability methods in identifying consistent motifs across genomic loci and predicting variant effects. The framework also enables quantification of epistatic interactions within and between regulatory elements and provides global mechanistic explanations across sequence contexts, advancing the mechanistic interpretation of genomic DNNs.</t>
+  </si>
+  <si>
+    <t>Here we introduce MAVE-NN, a neural-network-based Python package that implements a broadly applicable information-theoretic framework for learning genotype-phenotype maps—including biophysically interpretable models—from MAVE datasets. We demonstrate MAVE-NN in multiple biological contexts, and highlight the ability of our approach to deconvolve mutational effects from otherwise confounding experimental nonlinearities and noise.</t>
+  </si>
+  <si>
+    <t>This review examines how massively parallel assays—including deep mutational scanning, high-throughput SELEX, and massively parallel reporter assays—have transformed the quantitative modeling of sequence–function relationships across diverse biological contexts, from clinical variant interpretation to transcription factor binding, protein landscapes, and cis-regulatory mechanisms. We present a unified conceptual framework and core mathematical modeling strategies applicable across these areas, spanning topics such as protein evolution, transcriptional regulation, and mRNA splicing. We emphasize critical principles of experimental design and mathematical modeling necessary for ensuring interpretability and reproducibility in such studies.</t>
+  </si>
+  <si>
+    <t>Here we describe a field-theoretic approach that addresses this problem remarkably well in one dimension, providing an exact nonparametric Bayesian posterior without relying on tunable parameters or large-data approximations. Strong non-Gaussian constraints, which require a nonperturbative treatment, are found to play a major role in reducing distribution uncertainty. A software implementation of this method is provided.</t>
+  </si>
+  <si>
+    <t>Here we describe a new experimental approach, called Tite-Seq, that is capable of measuring binding titration curves and corresponding affinities for thousands of variant antibodies in parallel. The measurement of titration curves eliminates the confounding effects of antibody expression and stability that arise in standard deep mutational scanning assays.</t>
+  </si>
+  <si>
+    <t>This paper proposes a mathematical formalization of "equitability"—the ability to quantify statistical associations without bias toward specific relationship forms—using core concepts from information theory. We show that mutual information, a fundamental information-theoretic measure of dependence, naturally satisfies this equitability criterion, whereas the recently introduced maximal information coefficient violates it. We conclude that estimating mutual information provides a natural and practical method for equitably quantifying associations in large datasets.</t>
+  </si>
+  <si>
+    <t>/pictures/figures/fig1_deeplearning_kinney2010.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599AEEC6-9B2A-4372-AD73-EFDE8C26CA69}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1131,7 +1149,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1154,7 +1172,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1176,6 +1194,9 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1202,110 +1223,125 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
       </c>
       <c r="D6">
         <v>2022</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
       </c>
       <c r="D7">
         <v>2020</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
         <v>59</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
       </c>
       <c r="D8">
         <v>2019</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
         <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
       </c>
       <c r="D9">
         <v>2018</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
       </c>
       <c r="D10">
         <v>2016</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
         <v>54</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
       </c>
       <c r="D11">
         <v>2014</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1316,7 +1352,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>2010</v>
@@ -1325,10 +1361,10 @@
         <v>29</v>
       </c>
       <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
         <v>30</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add more figures for selected publications
</commit_message>
<xml_diff>
--- a/backend/selected_publications.xlsx
+++ b/backend/selected_publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aicorder\Documents\GitHub\aidancordero2.github.io\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C35D392-CCC1-488E-9265-365992444D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEBB85C-F8BD-49D6-812E-CD70FD037074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{5561A58E-8F97-4914-856A-96AEC28CEECE}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Title</t>
   </si>
@@ -79,9 +79,6 @@
     <t>https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1012818</t>
   </si>
   <si>
-    <t>/pictures/figures/fig1_gaugefixing_posfai_et_al.png</t>
-  </si>
-  <si>
     <t>Evan E Seitz, David M McCandlish, Justin B Kinney, Peter K Koo</t>
   </si>
   <si>
@@ -221,6 +218,27 @@
   </si>
   <si>
     <t>/pictures/figures/fig1_deeplearning_kinney2010.jpeg</t>
+  </si>
+  <si>
+    <t>/pictures/figures/fig1_gaugefixing_posfai_et_al.PNG</t>
+  </si>
+  <si>
+    <t>/pictures/figures/fig1_mavenn.png</t>
+  </si>
+  <si>
+    <t>/pictures/figures/fig1_mpra_review.png</t>
+  </si>
+  <si>
+    <t>/pictures/figures/fig1_density_estimation.png</t>
+  </si>
+  <si>
+    <t>/pictures/figures/fig1_tite_seq.png</t>
+  </si>
+  <si>
+    <t>/pictures/figures/fig1_equitability_kinney_2014.png</t>
+  </si>
+  <si>
+    <t>/pictures/figures/fig1_rousseau.png</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1113,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1148,8 +1166,11 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1169,10 +1190,10 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1180,22 +1201,22 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
       <c r="D4">
         <v>2024</v>
       </c>
       <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1203,145 +1224,160 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>2024</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
       </c>
       <c r="D6">
         <v>2022</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
         <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
       </c>
       <c r="D7">
         <v>2020</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
         <v>58</v>
-      </c>
-      <c r="G7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
       </c>
       <c r="D8">
         <v>2019</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
       </c>
       <c r="D9">
         <v>2018</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
         <v>49</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
       </c>
       <c r="D10">
         <v>2016</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
       </c>
       <c r="D11">
         <v>2014</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1352,19 +1388,19 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <v>2010</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
         <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update selected publication descriptions
</commit_message>
<xml_diff>
--- a/backend/selected_publications.xlsx
+++ b/backend/selected_publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aicorder\Documents\GitHub\aidancordero2.github.io\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEBB85C-F8BD-49D6-812E-CD70FD037074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BBA0D2-B609-44B6-86C7-F2EEE0D0A84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{5561A58E-8F97-4914-856A-96AEC28CEECE}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>Nature Communications 15 (1), 1880</t>
   </si>
   <si>
-    <t>Here, we introduce mechanistically interpretable quantitative models for how splice-modifying drugs work, combining massively parallel splicing assays, RNA-seq, and dose-response curves to characterize two SMA drugs, risdiplam and branaplam. The results reveal the sequence specificities of both drugs, suggest branaplam operates via two distinct interaction modes at 5' splice sites, and challenge the prevailing two-site hypothesis for risdiplam's activity at SMN2 exon 7. More broadly, the study finds that anomalous cooperativity and multi-drug synergy are widespread among exon-inclusion-promoting drugs, offering both mechanistic clarity on existing treatments and a framework for rational drug development.</t>
-  </si>
-  <si>
     <t>Yuma Ishigami, Mandy S Wong, Carlos Mart Gómez, Andalus Ayaz, Mahdi Kooshkbaghi, Sonya M Hanson, David M McCandlish, Adrian R Krainer, Justin B Kinney</t>
   </si>
   <si>
@@ -190,30 +187,18 @@
     <t>https://www.pnas.org/doi/10.1073/pnas.1309933111</t>
   </si>
   <si>
-    <t>This paper introduces an operator algebra framework that bridges two previously disconnected approaches to modeling multiparticle complexes in stochastic chemical systems: the statistical physics formalism (rooted in Doi's 1976 Fock space approach) and rule-based computational methods developed for simulating biochemical complexes. The new formalism extends Fock space to support not just particle creation and annihilation but also the assembly and disassembly of multiparticle complexes, with rules specified by algebraic operators via Wick's theorem and aided by diagrammatic tools. The result is a unified mathematical and computational framework applicable to both equilibrium and nonequilibrium systems, including a stochastic simulation algorithm for the latter.</t>
-  </si>
-  <si>
     <t>/pictures/figures/fig1_logomaker.png</t>
   </si>
   <si>
     <t>Here we introduce Logomaker, a Python API for creating publication-quality sequence logos. Logomaker can produce both standard and highly customized logos from either a matrix-like array of numbers or a multiple-sequence alignment. Logos are rendered as native matplotlib objects that are easy to stylize and incorporate into multi-panel figures.</t>
   </si>
   <si>
-    <t>This paper introduces SQUID (Surrogate Quantitative Interpretability for Deepnets), a framework for interpreting genomic deep neural networks by approximating them locally with simpler, inherently interpretable surrogate models that incorporate domain-specific knowledge about cis-regulatory mechanisms. By accounting for the confounding effects of nonlinearities and heteroscedastic noise in functional genomics data, SQUID outperforms existing interpretability methods in identifying consistent motifs across genomic loci and predicting variant effects. The framework also enables quantification of epistatic interactions within and between regulatory elements and provides global mechanistic explanations across sequence contexts, advancing the mechanistic interpretation of genomic DNNs.</t>
-  </si>
-  <si>
-    <t>Here we introduce MAVE-NN, a neural-network-based Python package that implements a broadly applicable information-theoretic framework for learning genotype-phenotype maps—including biophysically interpretable models—from MAVE datasets. We demonstrate MAVE-NN in multiple biological contexts, and highlight the ability of our approach to deconvolve mutational effects from otherwise confounding experimental nonlinearities and noise.</t>
-  </si>
-  <si>
     <t>This review examines how massively parallel assays—including deep mutational scanning, high-throughput SELEX, and massively parallel reporter assays—have transformed the quantitative modeling of sequence–function relationships across diverse biological contexts, from clinical variant interpretation to transcription factor binding, protein landscapes, and cis-regulatory mechanisms. We present a unified conceptual framework and core mathematical modeling strategies applicable across these areas, spanning topics such as protein evolution, transcriptional regulation, and mRNA splicing. We emphasize critical principles of experimental design and mathematical modeling necessary for ensuring interpretability and reproducibility in such studies.</t>
   </si>
   <si>
     <t>Here we describe a field-theoretic approach that addresses this problem remarkably well in one dimension, providing an exact nonparametric Bayesian posterior without relying on tunable parameters or large-data approximations. Strong non-Gaussian constraints, which require a nonperturbative treatment, are found to play a major role in reducing distribution uncertainty. A software implementation of this method is provided.</t>
   </si>
   <si>
-    <t>Here we describe a new experimental approach, called Tite-Seq, that is capable of measuring binding titration curves and corresponding affinities for thousands of variant antibodies in parallel. The measurement of titration curves eliminates the confounding effects of antibody expression and stability that arise in standard deep mutational scanning assays.</t>
-  </si>
-  <si>
     <t>This paper proposes a mathematical formalization of "equitability"—the ability to quantify statistical associations without bias toward specific relationship forms—using core concepts from information theory. We show that mutual information, a fundamental information-theoretic measure of dependence, naturally satisfies this equitability criterion, whereas the recently introduced maximal information coefficient violates it. We conclude that estimating mutual information provides a natural and practical method for equitably quantifying associations in large datasets.</t>
   </si>
   <si>
@@ -239,6 +224,21 @@
   </si>
   <si>
     <t>/pictures/figures/fig1_rousseau.png</t>
+  </si>
+  <si>
+    <t>Here, we introduce an operator algebra framework that bridges two previously disconnected approaches to modeling multiparticle complexes in stochastic chemical systems: the statistical physics formalism (rooted in Doi's 1976 Fock space approach) and rule-based computational methods developed for simulating biochemical complexes. The new formalism extends Fock space to support not just particle creation and annihilation but also the assembly and disassembly of multiparticle complexes, with rules specified by algebraic operators via Wick's theorem and aided by diagrammatic tools. The result is a unified mathematical and computational framework applicable to both equilibrium and nonequilibrium systems, including a stochastic simulation algorithm for the latter.</t>
+  </si>
+  <si>
+    <t>We introduce SQUID (Surrogate Quantitative Interpretability for Deepnets), a framework for interpreting genomic deep neural networks by approximating them locally with simpler, inherently interpretable surrogate models that incorporate domain-specific knowledge about cis-regulatory mechanisms. By accounting for the confounding effects of nonlinearities and heteroscedastic noise in functional genomics data, SQUID outperforms existing interpretability methods in identifying consistent motifs across genomic loci and predicting variant effects. The framework also enables quantification of epistatic interactions within and between regulatory elements and provides global mechanistic explanations across sequence contexts, advancing the mechanistic interpretation of genomic DNNs.</t>
+  </si>
+  <si>
+    <t>In this study, we demonstrate mechanistically interpretable quantitative models for how splice-modifying drugs work, combining massively parallel splicing assays, RNA-seq, and dose-response curves to characterize two SMA drugs, risdiplam and branaplam. Our results reveal the sequence specificities of both drugs, suggest branaplam operates via two distinct interaction modes at 5' splice sites, and challenge the prevailing two-site hypothesis for risdiplam's activity at SMN2 exon 7. More broadly, we find that anomalous cooperativity and multi-drug synergy are widespread among exon-inclusion-promoting drugs, offering both mechanistic clarity on existing treatments and a framework for rational drug development.</t>
+  </si>
+  <si>
+    <t>MAVE-NN is a neural-network-based Python package developed by the Kinney Lab that implements a broadly applicable information-theoretic framework for learning genotype-phenotype maps—including biophysically interpretable models—from MAVE datasets. We demonstrate MAVE-NN in multiple biological contexts, and highlight the ability of our approach to deconvolve mutational effects from otherwise confounding experimental nonlinearities and noise.</t>
+  </si>
+  <si>
+    <t>We describe a new experimental approach, called Tite-Seq, that is capable of measuring binding titration curves and corresponding affinities for thousands of variant antibodies in parallel. The measurement of titration curves eliminates the confounding effects of antibody expression and stability that arise in standard deep mutational scanning assays.</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1113,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1167,10 +1167,10 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1190,10 +1190,10 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1216,7 +1216,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1224,7 +1224,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -1233,151 +1233,151 @@
         <v>2024</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
       </c>
       <c r="D6">
         <v>2022</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
       </c>
       <c r="D7">
         <v>2020</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
       </c>
       <c r="D8">
         <v>2019</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
       </c>
       <c r="D9">
         <v>2018</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
       </c>
       <c r="D10">
         <v>2016</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
       </c>
       <c r="D11">
         <v>2014</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1388,19 +1388,19 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>2010</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
         <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>